<commit_message>
Added more species and Markdown file
Added the preliminary values for the four extra species of pterosaurs and created a markdown file containing the values used for the analyses.
</commit_message>
<xml_diff>
--- a/BEAST2/Ptero's/Data/Ptero ages.xlsx
+++ b/BEAST2/Ptero's/Data/Ptero ages.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\BEAST\XML's\Ptero's\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6BE4618-3095-490C-A465-8959A9730835}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EA46A3-2818-4B50-9AF8-CAEAEDB31DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D1360FA9-3365-40CC-8225-CD928C39C5E1}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="43">
   <si>
     <t>accepted_name</t>
   </si>
@@ -153,13 +153,25 @@
   </si>
   <si>
     <t>Y</t>
+  </si>
+  <si>
+    <t>Allkaruen koi</t>
+  </si>
+  <si>
+    <t>Cacibupteryx caribensis</t>
+  </si>
+  <si>
+    <t>Dimorphodon macronyx</t>
+  </si>
+  <si>
+    <t>Rhamphorhynchus muensteri</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,8 +203,14 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -247,8 +265,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -256,11 +286,26 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -281,6 +326,10 @@
     <xf numFmtId="0" fontId="3" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,10 +644,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D336B04-D74B-4DEC-B807-60D1529292D8}">
-  <dimension ref="A1:J50"/>
+  <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G38" sqref="G38"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="C58" sqref="C58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -652,14 +701,12 @@
         <v>204.9</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H2" s="2">
-        <v>216.65</v>
-      </c>
-      <c r="I2" s="15" t="s">
-        <v>38</v>
-      </c>
+        <v>204.9</v>
+      </c>
+      <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10">
@@ -708,7 +755,7 @@
         <v>216.65</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="H4" s="2">
         <v>216.65</v>
@@ -736,10 +783,10 @@
         <v>216.65</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="H5" s="2">
-        <v>208.8</v>
+        <v>216.65</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>38</v>
@@ -764,10 +811,10 @@
         <v>208.8</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="H6" s="2">
-        <v>217.25</v>
+        <v>208.8</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>38</v>
@@ -791,11 +838,11 @@
         <f t="shared" si="0"/>
         <v>217.25</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>8</v>
+      <c r="G7" s="3" t="s">
+        <v>5</v>
       </c>
       <c r="H7" s="2">
-        <v>210.35</v>
+        <v>217.25</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>38</v>
@@ -819,15 +866,13 @@
         <f t="shared" si="0"/>
         <v>212.25</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>8</v>
+      <c r="G8" s="3" t="s">
+        <v>6</v>
       </c>
       <c r="H8" s="2">
-        <v>210.35</v>
-      </c>
-      <c r="I8" s="15" t="s">
-        <v>38</v>
-      </c>
+        <v>212.25</v>
+      </c>
+      <c r="I8" s="2"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10">
@@ -848,14 +893,12 @@
         <v>225.5</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="H9" s="2">
         <v>225.5</v>
       </c>
-      <c r="I9" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="I9" s="2"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10">
@@ -875,11 +918,11 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G10" s="5" t="s">
-        <v>9</v>
+      <c r="G10" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H10" s="2">
-        <v>221</v>
+        <v>210.35</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>38</v>
@@ -903,11 +946,11 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G11" s="5" t="s">
-        <v>9</v>
+      <c r="G11" s="6" t="s">
+        <v>8</v>
       </c>
       <c r="H11" s="2">
-        <v>219.33999999999997</v>
+        <v>210.35</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>38</v>
@@ -931,11 +974,11 @@
         <f t="shared" si="0"/>
         <v>219.33999999999997</v>
       </c>
-      <c r="G12" s="6" t="s">
+      <c r="G12" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H12" s="2">
-        <v>217.75</v>
+        <v>225.5</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>38</v>
@@ -959,11 +1002,11 @@
         <f t="shared" si="0"/>
         <v>217.75</v>
       </c>
-      <c r="G13" s="6" t="s">
+      <c r="G13" s="5" t="s">
         <v>9</v>
       </c>
       <c r="H13" s="2">
-        <v>217.75</v>
+        <v>221</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>38</v>
@@ -988,10 +1031,10 @@
         <v>217.75</v>
       </c>
       <c r="G14" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="H14" s="2">
-        <v>225.5</v>
+        <v>219.33999999999997</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>38</v>
@@ -1015,11 +1058,11 @@
         <f t="shared" si="0"/>
         <v>221</v>
       </c>
-      <c r="G15" s="5" t="s">
-        <v>10</v>
+      <c r="G15" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="H15" s="2">
-        <v>213</v>
+        <v>217.75</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>38</v>
@@ -1043,11 +1086,11 @@
         <f t="shared" si="0"/>
         <v>225.5</v>
       </c>
-      <c r="G16" s="5" t="s">
-        <v>10</v>
+      <c r="G16" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="H16" s="2">
-        <v>211.89999999999998</v>
+        <v>217.75</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>38</v>
@@ -1075,7 +1118,7 @@
         <v>10</v>
       </c>
       <c r="H17" s="2">
-        <v>211.89999999999998</v>
+        <v>225.5</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>38</v>
@@ -1103,7 +1146,7 @@
         <v>10</v>
       </c>
       <c r="H18" s="2">
-        <v>209.75</v>
+        <v>213</v>
       </c>
       <c r="I18" s="15" t="s">
         <v>38</v>
@@ -1131,7 +1174,7 @@
         <v>10</v>
       </c>
       <c r="H19" s="2">
-        <v>209.75</v>
+        <v>211.89999999999998</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>38</v>
@@ -1159,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="H20" s="2">
-        <v>203.55</v>
+        <v>211.89999999999998</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>38</v>
@@ -1183,11 +1226,11 @@
         <f t="shared" si="0"/>
         <v>203.55</v>
       </c>
-      <c r="G21" s="3" t="s">
-        <v>11</v>
+      <c r="G21" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="H21" s="2">
-        <v>217.25</v>
+        <v>209.75</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>38</v>
@@ -1212,10 +1255,10 @@
         <v>209.75</v>
       </c>
       <c r="G22" s="5" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="H22" s="2">
-        <v>233.23000000000002</v>
+        <v>209.75</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>38</v>
@@ -1239,11 +1282,11 @@
         <f t="shared" si="0"/>
         <v>209.75</v>
       </c>
-      <c r="G23" s="6" t="s">
-        <v>15</v>
+      <c r="G23" s="5" t="s">
+        <v>10</v>
       </c>
       <c r="H23" s="2">
-        <v>238.25</v>
+        <v>203.55</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>38</v>
@@ -1267,11 +1310,11 @@
         <f t="shared" si="0"/>
         <v>217.25</v>
       </c>
-      <c r="G24" s="6" t="s">
-        <v>15</v>
+      <c r="G24" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="H24" s="2">
-        <v>238.25</v>
+        <v>217.25</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>38</v>
@@ -1296,12 +1339,12 @@
         <v>225.42000000000002</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="H25" s="2">
-        <v>235</v>
-      </c>
-      <c r="I25" s="15" t="s">
+        <v>225.42000000000002</v>
+      </c>
+      <c r="I25" s="17" t="s">
         <v>38</v>
       </c>
       <c r="J25" s="2"/>
@@ -1324,10 +1367,10 @@
         <v>233.23000000000002</v>
       </c>
       <c r="G26" s="5" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H26" s="2">
-        <v>235</v>
+        <v>233.23000000000002</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>38</v>
@@ -1351,15 +1394,13 @@
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
-      <c r="G27" s="5" t="s">
-        <v>17</v>
+      <c r="G27" s="3" t="s">
+        <v>14</v>
       </c>
       <c r="H27" s="2">
-        <v>235</v>
-      </c>
-      <c r="I27" s="15" t="s">
-        <v>38</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="I27" s="2"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10">
@@ -1379,11 +1420,11 @@
         <f t="shared" si="0"/>
         <v>238.25</v>
       </c>
-      <c r="G28" s="5" t="s">
-        <v>17</v>
+      <c r="G28" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="H28" s="2">
-        <v>235</v>
+        <v>238.25</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>38</v>
@@ -1407,11 +1448,11 @@
         <f t="shared" si="0"/>
         <v>238.25</v>
       </c>
-      <c r="G29" s="5" t="s">
-        <v>17</v>
+      <c r="G29" s="6" t="s">
+        <v>15</v>
       </c>
       <c r="H29" s="2">
-        <v>235</v>
+        <v>238.25</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>38</v>
@@ -1435,15 +1476,13 @@
         <f t="shared" si="0"/>
         <v>211.5</v>
       </c>
-      <c r="G30" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H30">
-        <v>217.25</v>
-      </c>
-      <c r="I30" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="G30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="H30" s="2">
+        <v>211.5</v>
+      </c>
+      <c r="I30" s="2"/>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10">
@@ -1463,13 +1502,13 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G31" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H31">
-        <v>216.8</v>
-      </c>
-      <c r="I31" s="16" t="s">
+      <c r="G31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" s="2">
+        <v>235</v>
+      </c>
+      <c r="I31" s="15" t="s">
         <v>38</v>
       </c>
       <c r="J31" s="2"/>
@@ -1491,13 +1530,13 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G32" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H32">
-        <v>216.8</v>
-      </c>
-      <c r="I32" s="16" t="s">
+      <c r="G32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" s="2">
+        <v>235</v>
+      </c>
+      <c r="I32" s="15" t="s">
         <v>38</v>
       </c>
       <c r="J32" s="2"/>
@@ -1520,12 +1559,12 @@
         <v>235</v>
       </c>
       <c r="G33" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H33">
-        <v>229.35</v>
-      </c>
-      <c r="I33" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H33" s="2">
+        <v>235</v>
+      </c>
+      <c r="I33" s="15" t="s">
         <v>38</v>
       </c>
       <c r="J33" s="2"/>
@@ -1547,13 +1586,13 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G34" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H34">
-        <v>212.25</v>
-      </c>
-      <c r="I34" s="16" t="s">
+      <c r="G34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="H34" s="2">
+        <v>235</v>
+      </c>
+      <c r="I34" s="15" t="s">
         <v>38</v>
       </c>
       <c r="J34" s="2"/>
@@ -1576,12 +1615,12 @@
         <v>235</v>
       </c>
       <c r="G35" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H35">
-        <v>230.48000000000002</v>
-      </c>
-      <c r="I35" s="16" t="s">
+        <v>17</v>
+      </c>
+      <c r="H35" s="2">
+        <v>235</v>
+      </c>
+      <c r="I35" s="15" t="s">
         <v>38</v>
       </c>
       <c r="J35" s="2"/>
@@ -1603,13 +1642,13 @@
         <f t="shared" si="0"/>
         <v>225.42000000000002</v>
       </c>
-      <c r="G36" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H36">
-        <v>217.4</v>
-      </c>
-      <c r="I36" s="16" t="s">
+      <c r="G36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="H36" s="2">
+        <v>225.42000000000002</v>
+      </c>
+      <c r="I36" s="17" t="s">
         <v>38</v>
       </c>
       <c r="J36" s="2"/>
@@ -1632,10 +1671,10 @@
         <v>212.25</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="H37" s="2">
-        <v>204.9</v>
+        <v>212.25</v>
       </c>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -1658,10 +1697,10 @@
         <v>209.3</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="H38" s="2">
-        <v>212.25</v>
+        <v>209.3</v>
       </c>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -1683,13 +1722,15 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G39" s="5" t="s">
-        <v>7</v>
+      <c r="G39" s="10" t="s">
+        <v>21</v>
       </c>
       <c r="H39" s="2">
-        <v>225.5</v>
-      </c>
-      <c r="I39" s="2"/>
+        <v>210.35</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>38</v>
+      </c>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10">
@@ -1709,11 +1750,11 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G40" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H40" s="2">
-        <v>225.42000000000002</v>
+      <c r="G40" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="H40">
+        <v>210.35</v>
       </c>
       <c r="I40" s="17" t="s">
         <v>38</v>
@@ -1737,12 +1778,14 @@
         <v>217.25</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H41" s="2">
-        <v>222</v>
-      </c>
-      <c r="I41" s="2"/>
+        <v>35</v>
+      </c>
+      <c r="H41">
+        <v>217.25</v>
+      </c>
+      <c r="I41" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="3" t="s">
@@ -1761,13 +1804,15 @@
         <f t="shared" si="0"/>
         <v>216.8</v>
       </c>
-      <c r="G42" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H42" s="2">
-        <v>211.5</v>
-      </c>
-      <c r="I42" s="2"/>
+      <c r="G42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H42">
+        <v>216.8</v>
+      </c>
+      <c r="I42" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="3" t="s">
@@ -1786,13 +1831,13 @@
         <f t="shared" si="0"/>
         <v>216.8</v>
       </c>
-      <c r="G43" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H43" s="2">
-        <v>225.42000000000002</v>
-      </c>
-      <c r="I43" s="17" t="s">
+      <c r="G43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H43">
+        <v>216.8</v>
+      </c>
+      <c r="I43" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1813,13 +1858,15 @@
         <f t="shared" si="0"/>
         <v>229.35</v>
       </c>
-      <c r="G44" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H44" s="2">
-        <v>212.25</v>
-      </c>
-      <c r="I44" s="2"/>
+      <c r="G44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H44">
+        <v>229.35</v>
+      </c>
+      <c r="I44" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="3" t="s">
@@ -1839,12 +1886,14 @@
         <v>212.25</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H45" s="2">
-        <v>209.3</v>
-      </c>
-      <c r="I45" s="2"/>
+        <v>25</v>
+      </c>
+      <c r="H45">
+        <v>212.25</v>
+      </c>
+      <c r="I45" s="16" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="5" t="s">
@@ -1863,13 +1912,13 @@
         <f t="shared" si="0"/>
         <v>230.48000000000002</v>
       </c>
-      <c r="G46" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H46" s="2">
-        <v>210.35</v>
-      </c>
-      <c r="I46" s="17" t="s">
+      <c r="G46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="H46">
+        <v>230.48000000000002</v>
+      </c>
+      <c r="I46" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1890,13 +1939,13 @@
         <f t="shared" si="0"/>
         <v>217.4</v>
       </c>
-      <c r="G47" s="10" t="s">
-        <v>21</v>
+      <c r="G47" s="3" t="s">
+        <v>27</v>
       </c>
       <c r="H47">
-        <v>210.35</v>
-      </c>
-      <c r="I47" s="17" t="s">
+        <v>217.4</v>
+      </c>
+      <c r="I47" s="16" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1951,7 +2000,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="50" spans="1:9">
+    <row r="50" spans="1:9" ht="15" thickBot="1">
       <c r="A50" s="10" t="s">
         <v>29</v>
       </c>
@@ -1978,10 +2027,67 @@
         <v>38</v>
       </c>
     </row>
+    <row r="51" spans="1:9" ht="15" thickBot="1">
+      <c r="A51" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="I51" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" ht="15" thickBot="1">
+      <c r="A52" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="I52" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" ht="15" thickBot="1">
+      <c r="A53" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="I53" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:9" ht="15" thickBot="1">
+      <c r="A54" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="I54" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:I50">
-    <sortCondition ref="I2:I50"/>
+    <sortCondition ref="G2:G50"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated folder names and Markdown
Updated folder names and made them match the names used in the markdown. Added new folder for next planned run.
</commit_message>
<xml_diff>
--- a/BEAST2/Ptero's/Data/Ptero ages.xlsx
+++ b/BEAST2/Ptero's/Data/Ptero ages.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68EA46A3-2818-4B50-9AF8-CAEAEDB31DAB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92AFAC2A-1586-4059-94AA-B8B71CF5D15B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D1360FA9-3365-40CC-8225-CD928C39C5E1}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Raw(ish) age data" sheetId="1" r:id="rId1"/>
+    <sheet name="Data for input into BEAST2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="258" uniqueCount="44">
   <si>
     <t>accepted_name</t>
   </si>
@@ -165,6 +166,9 @@
   </si>
   <si>
     <t>Rhamphorhynchus muensteri</t>
+  </si>
+  <si>
+    <t>Character data?</t>
   </si>
 </sst>
 </file>
@@ -210,7 +214,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="15">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -277,6 +281,24 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FF8DB5F8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -305,7 +327,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -330,6 +352,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -646,8 +676,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D336B04-D74B-4DEC-B807-60D1529292D8}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="C58" sqref="C58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -655,6 +685,7 @@
     <col min="1" max="1" width="26.6640625" customWidth="1"/>
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="4" width="8.77734375" customWidth="1"/>
+    <col min="6" max="6" width="15.88671875" customWidth="1"/>
     <col min="7" max="7" width="26.6640625" customWidth="1"/>
     <col min="8" max="10" width="12.33203125" customWidth="1"/>
   </cols>
@@ -672,15 +703,15 @@
       <c r="D1" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="2" t="s">
+      <c r="E1" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I1" s="2" t="s">
-        <v>37</v>
-      </c>
+      <c r="F1" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="G1" s="20"/>
+      <c r="H1" s="21"/>
+      <c r="I1" s="21"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10">
@@ -700,13 +731,10 @@
         <f>MEDIAN(C2,D2)</f>
         <v>204.9</v>
       </c>
-      <c r="G2" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="H2" s="2">
-        <v>204.9</v>
-      </c>
-      <c r="I2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="20"/>
+      <c r="H2" s="21"/>
+      <c r="I2" s="21"/>
       <c r="J2" s="2"/>
     </row>
     <row r="3" spans="1:10">
@@ -726,15 +754,12 @@
         <f t="shared" ref="E3:E50" si="0">MEDIAN(C3,D3)</f>
         <v>216.65</v>
       </c>
-      <c r="G3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3" s="2">
-        <v>216.65</v>
-      </c>
-      <c r="I3" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F3" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G3" s="20"/>
+      <c r="H3" s="21"/>
+      <c r="I3" s="21"/>
       <c r="J3" s="2"/>
     </row>
     <row r="4" spans="1:10">
@@ -754,15 +779,12 @@
         <f t="shared" si="0"/>
         <v>216.65</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4" s="2">
-        <v>216.65</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F4" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="21"/>
+      <c r="I4" s="21"/>
       <c r="J4" s="2"/>
     </row>
     <row r="5" spans="1:10">
@@ -782,15 +804,12 @@
         <f t="shared" si="0"/>
         <v>216.65</v>
       </c>
-      <c r="G5" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="H5" s="2">
-        <v>216.65</v>
-      </c>
-      <c r="I5" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F5" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
       <c r="J5" s="2"/>
     </row>
     <row r="6" spans="1:10">
@@ -810,15 +829,12 @@
         <f t="shared" si="0"/>
         <v>208.8</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="H6" s="2">
-        <v>208.8</v>
-      </c>
-      <c r="I6" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F6" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G6" s="20"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
       <c r="J6" s="2"/>
     </row>
     <row r="7" spans="1:10">
@@ -838,15 +854,12 @@
         <f t="shared" si="0"/>
         <v>217.25</v>
       </c>
-      <c r="G7" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="2">
-        <v>217.25</v>
-      </c>
-      <c r="I7" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="20"/>
+      <c r="H7" s="21"/>
+      <c r="I7" s="21"/>
       <c r="J7" s="2"/>
     </row>
     <row r="8" spans="1:10">
@@ -866,13 +879,10 @@
         <f t="shared" si="0"/>
         <v>212.25</v>
       </c>
-      <c r="G8" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="H8" s="2">
-        <v>212.25</v>
-      </c>
-      <c r="I8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="20"/>
+      <c r="H8" s="21"/>
+      <c r="I8" s="21"/>
       <c r="J8" s="2"/>
     </row>
     <row r="9" spans="1:10">
@@ -892,13 +902,10 @@
         <f t="shared" si="0"/>
         <v>225.5</v>
       </c>
-      <c r="G9" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="H9" s="2">
-        <v>225.5</v>
-      </c>
-      <c r="I9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="20"/>
+      <c r="H9" s="21"/>
+      <c r="I9" s="21"/>
       <c r="J9" s="2"/>
     </row>
     <row r="10" spans="1:10">
@@ -918,15 +925,12 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10" s="2">
-        <v>210.35</v>
-      </c>
-      <c r="I10" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F10" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G10" s="22"/>
+      <c r="H10" s="21"/>
+      <c r="I10" s="21"/>
       <c r="J10" s="2"/>
     </row>
     <row r="11" spans="1:10">
@@ -946,15 +950,12 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="H11" s="2">
-        <v>210.35</v>
-      </c>
-      <c r="I11" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F11" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G11" s="22"/>
+      <c r="H11" s="21"/>
+      <c r="I11" s="21"/>
       <c r="J11" s="2"/>
     </row>
     <row r="12" spans="1:10">
@@ -974,15 +975,12 @@
         <f t="shared" si="0"/>
         <v>219.33999999999997</v>
       </c>
-      <c r="G12" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H12" s="2">
-        <v>225.5</v>
-      </c>
-      <c r="I12" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F12" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
+      <c r="I12" s="21"/>
       <c r="J12" s="2"/>
     </row>
     <row r="13" spans="1:10">
@@ -1002,15 +1000,12 @@
         <f t="shared" si="0"/>
         <v>217.75</v>
       </c>
-      <c r="G13" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H13" s="2">
-        <v>221</v>
-      </c>
-      <c r="I13" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F13" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
+      <c r="I13" s="21"/>
       <c r="J13" s="2"/>
     </row>
     <row r="14" spans="1:10">
@@ -1030,15 +1025,12 @@
         <f t="shared" si="0"/>
         <v>217.75</v>
       </c>
-      <c r="G14" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="H14" s="2">
-        <v>219.33999999999997</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G14" s="20"/>
+      <c r="H14" s="21"/>
+      <c r="I14" s="21"/>
       <c r="J14" s="2"/>
     </row>
     <row r="15" spans="1:10">
@@ -1058,15 +1050,12 @@
         <f t="shared" si="0"/>
         <v>221</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H15" s="2">
-        <v>217.75</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F15" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G15" s="22"/>
+      <c r="H15" s="21"/>
+      <c r="I15" s="21"/>
       <c r="J15" s="2"/>
     </row>
     <row r="16" spans="1:10">
@@ -1086,15 +1075,12 @@
         <f t="shared" si="0"/>
         <v>225.5</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>9</v>
-      </c>
-      <c r="H16" s="2">
-        <v>217.75</v>
-      </c>
-      <c r="I16" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F16" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G16" s="22"/>
+      <c r="H16" s="21"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="2"/>
     </row>
     <row r="17" spans="1:10">
@@ -1114,15 +1100,12 @@
         <f t="shared" si="0"/>
         <v>211.89999999999998</v>
       </c>
-      <c r="G17" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H17" s="2">
-        <v>225.5</v>
-      </c>
-      <c r="I17" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F17" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G17" s="20"/>
+      <c r="H17" s="21"/>
+      <c r="I17" s="21"/>
       <c r="J17" s="2"/>
     </row>
     <row r="18" spans="1:10">
@@ -1142,15 +1125,12 @@
         <f t="shared" si="0"/>
         <v>211.89999999999998</v>
       </c>
-      <c r="G18" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H18" s="2">
-        <v>213</v>
-      </c>
-      <c r="I18" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F18" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G18" s="20"/>
+      <c r="H18" s="21"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="2"/>
     </row>
     <row r="19" spans="1:10">
@@ -1170,15 +1150,12 @@
         <f t="shared" si="0"/>
         <v>225.5</v>
       </c>
-      <c r="G19" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H19" s="2">
-        <v>211.89999999999998</v>
-      </c>
-      <c r="I19" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F19" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G19" s="20"/>
+      <c r="H19" s="21"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="2"/>
     </row>
     <row r="20" spans="1:10">
@@ -1198,15 +1175,12 @@
         <f t="shared" si="0"/>
         <v>213</v>
       </c>
-      <c r="G20" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H20" s="2">
-        <v>211.89999999999998</v>
-      </c>
-      <c r="I20" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F20" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G20" s="20"/>
+      <c r="H20" s="21"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="2"/>
     </row>
     <row r="21" spans="1:10">
@@ -1226,15 +1200,12 @@
         <f t="shared" si="0"/>
         <v>203.55</v>
       </c>
-      <c r="G21" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H21" s="2">
-        <v>209.75</v>
-      </c>
-      <c r="I21" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F21" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G21" s="20"/>
+      <c r="H21" s="21"/>
+      <c r="I21" s="21"/>
       <c r="J21" s="2"/>
     </row>
     <row r="22" spans="1:10">
@@ -1254,15 +1225,12 @@
         <f t="shared" si="0"/>
         <v>209.75</v>
       </c>
-      <c r="G22" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H22" s="2">
-        <v>209.75</v>
-      </c>
-      <c r="I22" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F22" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G22" s="20"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="2"/>
     </row>
     <row r="23" spans="1:10">
@@ -1282,15 +1250,12 @@
         <f t="shared" si="0"/>
         <v>209.75</v>
       </c>
-      <c r="G23" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H23" s="2">
-        <v>203.55</v>
-      </c>
-      <c r="I23" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F23" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G23" s="20"/>
+      <c r="H23" s="21"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="2"/>
     </row>
     <row r="24" spans="1:10">
@@ -1310,15 +1275,12 @@
         <f t="shared" si="0"/>
         <v>217.25</v>
       </c>
-      <c r="G24" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H24" s="2">
-        <v>217.25</v>
-      </c>
-      <c r="I24" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F24" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G24" s="20"/>
+      <c r="H24" s="21"/>
+      <c r="I24" s="21"/>
       <c r="J24" s="2"/>
     </row>
     <row r="25" spans="1:10">
@@ -1338,15 +1300,12 @@
         <f t="shared" si="0"/>
         <v>225.42000000000002</v>
       </c>
-      <c r="G25" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="H25" s="2">
-        <v>225.42000000000002</v>
-      </c>
-      <c r="I25" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="F25" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G25" s="20"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="23"/>
       <c r="J25" s="2"/>
     </row>
     <row r="26" spans="1:10">
@@ -1366,15 +1325,12 @@
         <f t="shared" si="0"/>
         <v>233.23000000000002</v>
       </c>
-      <c r="G26" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="H26" s="2">
-        <v>233.23000000000002</v>
-      </c>
-      <c r="I26" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F26" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G26" s="20"/>
+      <c r="H26" s="21"/>
+      <c r="I26" s="21"/>
       <c r="J26" s="2"/>
     </row>
     <row r="27" spans="1:10">
@@ -1394,13 +1350,10 @@
         <f t="shared" si="0"/>
         <v>222</v>
       </c>
-      <c r="G27" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="H27" s="2">
-        <v>222</v>
-      </c>
-      <c r="I27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="21"/>
+      <c r="I27" s="21"/>
       <c r="J27" s="2"/>
     </row>
     <row r="28" spans="1:10">
@@ -1420,15 +1373,12 @@
         <f t="shared" si="0"/>
         <v>238.25</v>
       </c>
-      <c r="G28" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H28" s="2">
-        <v>238.25</v>
-      </c>
-      <c r="I28" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F28" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G28" s="22"/>
+      <c r="H28" s="21"/>
+      <c r="I28" s="21"/>
       <c r="J28" s="2"/>
     </row>
     <row r="29" spans="1:10">
@@ -1448,15 +1398,12 @@
         <f t="shared" si="0"/>
         <v>238.25</v>
       </c>
-      <c r="G29" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="H29" s="2">
-        <v>238.25</v>
-      </c>
-      <c r="I29" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F29" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="22"/>
+      <c r="H29" s="21"/>
+      <c r="I29" s="21"/>
       <c r="J29" s="2"/>
     </row>
     <row r="30" spans="1:10">
@@ -1476,13 +1423,10 @@
         <f t="shared" si="0"/>
         <v>211.5</v>
       </c>
-      <c r="G30" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="H30" s="2">
-        <v>211.5</v>
-      </c>
-      <c r="I30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="21"/>
+      <c r="I30" s="21"/>
       <c r="J30" s="2"/>
     </row>
     <row r="31" spans="1:10">
@@ -1502,15 +1446,12 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G31" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H31" s="2">
-        <v>235</v>
-      </c>
-      <c r="I31" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F31" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G31" s="20"/>
+      <c r="H31" s="21"/>
+      <c r="I31" s="21"/>
       <c r="J31" s="2"/>
     </row>
     <row r="32" spans="1:10">
@@ -1530,15 +1471,12 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G32" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H32" s="2">
-        <v>235</v>
-      </c>
-      <c r="I32" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F32" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G32" s="20"/>
+      <c r="H32" s="21"/>
+      <c r="I32" s="21"/>
       <c r="J32" s="2"/>
     </row>
     <row r="33" spans="1:10">
@@ -1558,15 +1496,12 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G33" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H33" s="2">
-        <v>235</v>
-      </c>
-      <c r="I33" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F33" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="20"/>
+      <c r="H33" s="21"/>
+      <c r="I33" s="21"/>
       <c r="J33" s="2"/>
     </row>
     <row r="34" spans="1:10">
@@ -1586,15 +1521,12 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G34" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H34" s="2">
-        <v>235</v>
-      </c>
-      <c r="I34" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F34" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G34" s="20"/>
+      <c r="H34" s="21"/>
+      <c r="I34" s="21"/>
       <c r="J34" s="2"/>
     </row>
     <row r="35" spans="1:10">
@@ -1614,15 +1546,12 @@
         <f t="shared" si="0"/>
         <v>235</v>
       </c>
-      <c r="G35" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="H35" s="2">
-        <v>235</v>
-      </c>
-      <c r="I35" s="15" t="s">
-        <v>38</v>
-      </c>
+      <c r="F35" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G35" s="20"/>
+      <c r="H35" s="21"/>
+      <c r="I35" s="21"/>
       <c r="J35" s="2"/>
     </row>
     <row r="36" spans="1:10">
@@ -1642,15 +1571,12 @@
         <f t="shared" si="0"/>
         <v>225.42000000000002</v>
       </c>
-      <c r="G36" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="H36" s="2">
-        <v>225.42000000000002</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="F36" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G36" s="24"/>
+      <c r="H36" s="21"/>
+      <c r="I36" s="23"/>
       <c r="J36" s="2"/>
     </row>
     <row r="37" spans="1:10">
@@ -1670,13 +1596,10 @@
         <f t="shared" si="0"/>
         <v>212.25</v>
       </c>
-      <c r="G37" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H37" s="2">
-        <v>212.25</v>
-      </c>
-      <c r="I37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="20"/>
+      <c r="H37" s="21"/>
+      <c r="I37" s="21"/>
       <c r="J37" s="2"/>
     </row>
     <row r="38" spans="1:10">
@@ -1696,13 +1619,10 @@
         <f t="shared" si="0"/>
         <v>209.3</v>
       </c>
-      <c r="G38" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="H38" s="2">
-        <v>209.3</v>
-      </c>
-      <c r="I38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="20"/>
+      <c r="H38" s="21"/>
+      <c r="I38" s="21"/>
       <c r="J38" s="2"/>
     </row>
     <row r="39" spans="1:10">
@@ -1722,15 +1642,12 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G39" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H39" s="2">
-        <v>210.35</v>
-      </c>
-      <c r="I39" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="F39" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G39" s="22"/>
+      <c r="H39" s="21"/>
+      <c r="I39" s="23"/>
       <c r="J39" s="2"/>
     </row>
     <row r="40" spans="1:10">
@@ -1750,15 +1667,12 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G40" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="H40">
-        <v>210.35</v>
-      </c>
-      <c r="I40" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="F40" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G40" s="22"/>
+      <c r="H40" s="23"/>
+      <c r="I40" s="23"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="3" t="s">
@@ -1777,15 +1691,12 @@
         <f t="shared" si="0"/>
         <v>217.25</v>
       </c>
-      <c r="G41" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="H41">
-        <v>217.25</v>
-      </c>
-      <c r="I41" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="F41" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G41" s="20"/>
+      <c r="H41" s="23"/>
+      <c r="I41" s="23"/>
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="3" t="s">
@@ -1804,15 +1715,12 @@
         <f t="shared" si="0"/>
         <v>216.8</v>
       </c>
-      <c r="G42" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H42">
-        <v>216.8</v>
-      </c>
-      <c r="I42" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="F42" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G42" s="20"/>
+      <c r="H42" s="23"/>
+      <c r="I42" s="23"/>
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="3" t="s">
@@ -1831,15 +1739,12 @@
         <f t="shared" si="0"/>
         <v>216.8</v>
       </c>
-      <c r="G43" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H43">
-        <v>216.8</v>
-      </c>
-      <c r="I43" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="F43" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G43" s="20"/>
+      <c r="H43" s="23"/>
+      <c r="I43" s="23"/>
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="5" t="s">
@@ -1858,15 +1763,12 @@
         <f t="shared" si="0"/>
         <v>229.35</v>
       </c>
-      <c r="G44" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="H44">
-        <v>229.35</v>
-      </c>
-      <c r="I44" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="F44" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G44" s="20"/>
+      <c r="H44" s="23"/>
+      <c r="I44" s="23"/>
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="3" t="s">
@@ -1885,15 +1787,12 @@
         <f t="shared" si="0"/>
         <v>212.25</v>
       </c>
-      <c r="G45" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H45">
-        <v>212.25</v>
-      </c>
-      <c r="I45" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="F45" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G45" s="20"/>
+      <c r="H45" s="23"/>
+      <c r="I45" s="23"/>
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="5" t="s">
@@ -1912,15 +1811,12 @@
         <f t="shared" si="0"/>
         <v>230.48000000000002</v>
       </c>
-      <c r="G46" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H46">
-        <v>230.48000000000002</v>
-      </c>
-      <c r="I46" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="F46" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G46" s="20"/>
+      <c r="H46" s="23"/>
+      <c r="I46" s="23"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="3" t="s">
@@ -1939,15 +1835,12 @@
         <f t="shared" si="0"/>
         <v>217.4</v>
       </c>
-      <c r="G47" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="H47">
-        <v>217.4</v>
-      </c>
-      <c r="I47" s="16" t="s">
-        <v>38</v>
-      </c>
+      <c r="F47" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="G47" s="20"/>
+      <c r="H47" s="23"/>
+      <c r="I47" s="23"/>
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="3" t="s">
@@ -1966,12 +1859,9 @@
         <f t="shared" si="0"/>
         <v>220.55799999999999</v>
       </c>
-      <c r="G48" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="H48">
-        <v>220.55799999999999</v>
-      </c>
+      <c r="G48" s="20"/>
+      <c r="H48" s="23"/>
+      <c r="I48" s="23"/>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="10" t="s">
@@ -1990,15 +1880,12 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G49" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H49">
-        <v>210.35</v>
-      </c>
-      <c r="I49" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="F49" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G49" s="22"/>
+      <c r="H49" s="23"/>
+      <c r="I49" s="23"/>
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1">
       <c r="A50" s="10" t="s">
@@ -2017,15 +1904,12 @@
         <f t="shared" si="0"/>
         <v>210.35</v>
       </c>
-      <c r="G50" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="H50">
-        <v>210.35</v>
-      </c>
-      <c r="I50" s="17" t="s">
-        <v>38</v>
-      </c>
+      <c r="F50" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="G50" s="22"/>
+      <c r="H50" s="23"/>
+      <c r="I50" s="23"/>
     </row>
     <row r="51" spans="1:9" ht="15" thickBot="1">
       <c r="A51" s="18" t="s">
@@ -2034,12 +1918,12 @@
       <c r="B51" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G51" s="18" t="s">
-        <v>39</v>
-      </c>
-      <c r="I51" s="19" t="s">
-        <v>38</v>
-      </c>
+      <c r="F51" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G51" s="25"/>
+      <c r="H51" s="23"/>
+      <c r="I51" s="23"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1">
       <c r="A52" s="18" t="s">
@@ -2048,12 +1932,12 @@
       <c r="B52" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G52" s="18" t="s">
-        <v>40</v>
-      </c>
-      <c r="I52" s="19" t="s">
-        <v>38</v>
-      </c>
+      <c r="F52" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G52" s="25"/>
+      <c r="H52" s="23"/>
+      <c r="I52" s="23"/>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1">
       <c r="A53" s="18" t="s">
@@ -2062,12 +1946,12 @@
       <c r="B53" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G53" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="I53" s="19" t="s">
-        <v>38</v>
-      </c>
+      <c r="F53" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" s="25"/>
+      <c r="H53" s="23"/>
+      <c r="I53" s="23"/>
     </row>
     <row r="54" spans="1:9" ht="15" thickBot="1">
       <c r="A54" s="18" t="s">
@@ -2076,12 +1960,12 @@
       <c r="B54" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="G54" s="18" t="s">
-        <v>42</v>
-      </c>
-      <c r="I54" s="19" t="s">
-        <v>38</v>
-      </c>
+      <c r="F54" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="G54" s="25"/>
+      <c r="H54" s="23"/>
+      <c r="I54" s="23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:I50">
@@ -2090,4 +1974,587 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9851237-01A2-4A74-AEF5-AB1CB64C8E21}">
+  <dimension ref="A1:C54"/>
+  <sheetViews>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="25.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>204.9</v>
+      </c>
+      <c r="C2" s="2"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>216.65</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="2">
+        <v>216.65</v>
+      </c>
+      <c r="C4" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" s="2">
+        <v>216.65</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2">
+        <v>208.8</v>
+      </c>
+      <c r="C6" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="2">
+        <v>217.25</v>
+      </c>
+      <c r="C7" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="2">
+        <v>212.25</v>
+      </c>
+      <c r="C8" s="2"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" s="2">
+        <v>225.5</v>
+      </c>
+      <c r="C9" s="2"/>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2">
+        <v>210.35</v>
+      </c>
+      <c r="C10" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2">
+        <v>210.35</v>
+      </c>
+      <c r="C11" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2">
+        <v>225.5</v>
+      </c>
+      <c r="C12" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2">
+        <v>221</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2">
+        <v>219.33999999999997</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2">
+        <v>217.75</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2">
+        <v>217.75</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B17" s="2">
+        <v>225.5</v>
+      </c>
+      <c r="C17" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="2">
+        <v>213</v>
+      </c>
+      <c r="C18" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B19" s="2">
+        <v>211.89999999999998</v>
+      </c>
+      <c r="C19" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B20" s="2">
+        <v>211.89999999999998</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B21" s="2">
+        <v>209.75</v>
+      </c>
+      <c r="C21" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="2">
+        <v>209.75</v>
+      </c>
+      <c r="C22" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" s="2">
+        <v>203.55</v>
+      </c>
+      <c r="C23" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B24" s="2">
+        <v>217.25</v>
+      </c>
+      <c r="C24" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B25" s="2">
+        <v>225.42000000000002</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B26" s="2">
+        <v>233.23000000000002</v>
+      </c>
+      <c r="C26" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B27" s="2">
+        <v>222</v>
+      </c>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="2">
+        <v>238.25</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="2">
+        <v>238.25</v>
+      </c>
+      <c r="C29" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="2">
+        <v>211.5</v>
+      </c>
+      <c r="C30" s="2"/>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="2">
+        <v>235</v>
+      </c>
+      <c r="C31" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B32" s="2">
+        <v>235</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B33" s="2">
+        <v>235</v>
+      </c>
+      <c r="C33" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B34" s="2">
+        <v>235</v>
+      </c>
+      <c r="C34" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B35" s="2">
+        <v>235</v>
+      </c>
+      <c r="C35" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="B36" s="2">
+        <v>225.42000000000002</v>
+      </c>
+      <c r="C36" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="2">
+        <v>212.25</v>
+      </c>
+      <c r="C37" s="2"/>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B38" s="2">
+        <v>209.3</v>
+      </c>
+      <c r="C38" s="2"/>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B39" s="2">
+        <v>210.35</v>
+      </c>
+      <c r="C39" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B40">
+        <v>210.35</v>
+      </c>
+      <c r="C40" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B41">
+        <v>217.25</v>
+      </c>
+      <c r="C41" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B42">
+        <v>216.8</v>
+      </c>
+      <c r="C42" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B43">
+        <v>216.8</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="A44" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B44">
+        <v>229.35</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="A45" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B45">
+        <v>212.25</v>
+      </c>
+      <c r="C45" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3">
+      <c r="A46" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B46">
+        <v>230.48000000000002</v>
+      </c>
+      <c r="C46" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3">
+      <c r="A47" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B47">
+        <v>217.4</v>
+      </c>
+      <c r="C47" s="16" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3">
+      <c r="A48" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="B48">
+        <v>220.55799999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3">
+      <c r="A49" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B49">
+        <v>210.35</v>
+      </c>
+      <c r="C49" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" ht="15" thickBot="1">
+      <c r="A50" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="B50">
+        <v>210.35</v>
+      </c>
+      <c r="C50" s="17" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="15" thickBot="1">
+      <c r="A51" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C51" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" ht="15" thickBot="1">
+      <c r="A52" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="C52" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="15" thickBot="1">
+      <c r="A53" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="C53" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" ht="15" thickBot="1">
+      <c r="A54" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="C54" s="19" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Update after particle error
Update with all the files after the new Particle error
</commit_message>
<xml_diff>
--- a/BEAST2/Ptero's/Data/Ptero ages.xlsx
+++ b/BEAST2/Ptero's/Data/Ptero ages.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B47BDA-86D3-439E-A8F7-B46E04B0EC73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82489493-58B3-4AD3-AD4A-BD5C1966954A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{D1360FA9-3365-40CC-8225-CD928C39C5E1}"/>
   </bookViews>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="330" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="46">
   <si>
     <t>accepted_name</t>
   </si>
@@ -104,9 +104,6 @@
   </si>
   <si>
     <t>Pachagnathus benitoi</t>
-  </si>
-  <si>
-    <t>Peteinosaurus zambelli</t>
   </si>
   <si>
     <t>Preondactylus buffarinii</t>
@@ -337,7 +334,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -370,9 +367,6 @@
     <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,8 +683,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D336B04-D74B-4DEC-B807-60D1529292D8}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F1" activeCellId="5" sqref="A1:A1048576 B1:B1048576 C1:C1048576 D1:D1048576 E1:E1048576 F1:F1048576"/>
+    <sheetView topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="H48" sqref="H48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -708,19 +702,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G1" s="20"/>
       <c r="H1" s="21"/>
@@ -732,7 +726,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="4">
         <v>208.5</v>
@@ -755,7 +749,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="3">
         <v>217.8</v>
@@ -768,7 +762,7 @@
         <v>216.65</v>
       </c>
       <c r="F3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G3" s="20"/>
       <c r="H3" s="21"/>
@@ -780,7 +774,7 @@
         <v>2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7">
         <v>217.8</v>
@@ -793,7 +787,7 @@
         <v>216.65</v>
       </c>
       <c r="F4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="21"/>
@@ -805,7 +799,7 @@
         <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="7">
         <v>217.8</v>
@@ -818,7 +812,7 @@
         <v>216.65</v>
       </c>
       <c r="F5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="21"/>
@@ -830,7 +824,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6" s="7">
         <v>216.3</v>
@@ -843,7 +837,7 @@
         <v>208.8</v>
       </c>
       <c r="F6" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="21"/>
@@ -855,7 +849,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C7" s="7">
         <v>218.5</v>
@@ -868,7 +862,7 @@
         <v>217.25</v>
       </c>
       <c r="F7" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="21"/>
@@ -880,7 +874,7 @@
         <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C8" s="7">
         <v>216</v>
@@ -903,7 +897,7 @@
         <v>7</v>
       </c>
       <c r="B9" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C9" s="8">
         <v>227</v>
@@ -926,7 +920,7 @@
         <v>8</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="9">
         <v>214.7</v>
@@ -939,7 +933,7 @@
         <v>210.35</v>
       </c>
       <c r="F10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G10" s="22"/>
       <c r="H10" s="21"/>
@@ -951,7 +945,7 @@
         <v>8</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="9">
         <v>214.7</v>
@@ -964,7 +958,7 @@
         <v>210.35</v>
       </c>
       <c r="F11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G11" s="22"/>
       <c r="H11" s="21"/>
@@ -976,7 +970,7 @@
         <v>9</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="8">
         <v>219.45</v>
@@ -989,7 +983,7 @@
         <v>219.33999999999997</v>
       </c>
       <c r="F12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G12" s="20"/>
       <c r="H12" s="21"/>
@@ -1001,7 +995,7 @@
         <v>9</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="9">
         <v>227</v>
@@ -1014,7 +1008,7 @@
         <v>217.75</v>
       </c>
       <c r="F13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G13" s="20"/>
       <c r="H13" s="21"/>
@@ -1026,7 +1020,7 @@
         <v>9</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="9">
         <v>227</v>
@@ -1039,7 +1033,7 @@
         <v>217.75</v>
       </c>
       <c r="F14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G14" s="20"/>
       <c r="H14" s="21"/>
@@ -1051,7 +1045,7 @@
         <v>9</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C15" s="8">
         <v>227</v>
@@ -1064,7 +1058,7 @@
         <v>221</v>
       </c>
       <c r="F15" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G15" s="22"/>
       <c r="H15" s="21"/>
@@ -1076,7 +1070,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C16" s="8">
         <v>226</v>
@@ -1089,7 +1083,7 @@
         <v>225.5</v>
       </c>
       <c r="F16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G16" s="22"/>
       <c r="H16" s="21"/>
@@ -1101,7 +1095,7 @@
         <v>10</v>
       </c>
       <c r="B17" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C17" s="8">
         <v>212.6</v>
@@ -1114,7 +1108,7 @@
         <v>211.89999999999998</v>
       </c>
       <c r="F17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G17" s="20"/>
       <c r="H17" s="21"/>
@@ -1126,7 +1120,7 @@
         <v>10</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="8">
         <v>212.6</v>
@@ -1139,7 +1133,7 @@
         <v>211.89999999999998</v>
       </c>
       <c r="F18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G18" s="20"/>
       <c r="H18" s="21"/>
@@ -1151,7 +1145,7 @@
         <v>10</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C19" s="8">
         <v>226</v>
@@ -1164,7 +1158,7 @@
         <v>225.5</v>
       </c>
       <c r="F19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G19" s="20"/>
       <c r="H19" s="21"/>
@@ -1176,7 +1170,7 @@
         <v>10</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="8">
         <v>215</v>
@@ -1189,7 +1183,7 @@
         <v>213</v>
       </c>
       <c r="F20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G20" s="20"/>
       <c r="H20" s="21"/>
@@ -1201,7 +1195,7 @@
         <v>10</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C21" s="8">
         <v>204.1</v>
@@ -1214,7 +1208,7 @@
         <v>203.55</v>
       </c>
       <c r="F21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G21" s="20"/>
       <c r="H21" s="21"/>
@@ -1226,7 +1220,7 @@
         <v>10</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C22" s="8">
         <v>211</v>
@@ -1239,7 +1233,7 @@
         <v>209.75</v>
       </c>
       <c r="F22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G22" s="20"/>
       <c r="H22" s="21"/>
@@ -1251,7 +1245,7 @@
         <v>10</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C23" s="8">
         <v>211</v>
@@ -1264,7 +1258,7 @@
         <v>209.75</v>
       </c>
       <c r="F23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="21"/>
@@ -1276,7 +1270,7 @@
         <v>11</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C24" s="7">
         <v>218.2</v>
@@ -1289,7 +1283,7 @@
         <v>217.25</v>
       </c>
       <c r="F24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
@@ -1301,7 +1295,7 @@
         <v>12</v>
       </c>
       <c r="B25" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C25" s="8">
         <v>225.79</v>
@@ -1314,7 +1308,7 @@
         <v>225.42000000000002</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="21"/>
@@ -1326,7 +1320,7 @@
         <v>13</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" s="8">
         <v>233.96</v>
@@ -1339,7 +1333,7 @@
         <v>233.23000000000002</v>
       </c>
       <c r="F26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
@@ -1351,7 +1345,7 @@
         <v>14</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C27" s="7">
         <v>224</v>
@@ -1374,7 +1368,7 @@
         <v>15</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C28" s="9">
         <v>239.5</v>
@@ -1387,7 +1381,7 @@
         <v>238.25</v>
       </c>
       <c r="F28" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G28" s="22"/>
       <c r="H28" s="21"/>
@@ -1399,7 +1393,7 @@
         <v>15</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C29" s="9">
         <v>239.5</v>
@@ -1412,7 +1406,7 @@
         <v>238.25</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G29" s="22"/>
       <c r="H29" s="21"/>
@@ -1424,7 +1418,7 @@
         <v>16</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" s="8">
         <v>213.1</v>
@@ -1447,7 +1441,7 @@
         <v>17</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C31" s="8">
         <v>236.7</v>
@@ -1460,7 +1454,7 @@
         <v>235</v>
       </c>
       <c r="F31" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G31" s="20"/>
       <c r="H31" s="21"/>
@@ -1472,7 +1466,7 @@
         <v>17</v>
       </c>
       <c r="B32" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C32" s="8">
         <v>236.7</v>
@@ -1485,7 +1479,7 @@
         <v>235</v>
       </c>
       <c r="F32" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G32" s="20"/>
       <c r="H32" s="21"/>
@@ -1497,7 +1491,7 @@
         <v>17</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C33" s="8">
         <v>236.7</v>
@@ -1510,7 +1504,7 @@
         <v>235</v>
       </c>
       <c r="F33" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G33" s="20"/>
       <c r="H33" s="21"/>
@@ -1522,7 +1516,7 @@
         <v>17</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="8">
         <v>236.7</v>
@@ -1535,7 +1529,7 @@
         <v>235</v>
       </c>
       <c r="F34" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G34" s="20"/>
       <c r="H34" s="21"/>
@@ -1547,7 +1541,7 @@
         <v>17</v>
       </c>
       <c r="B35" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C35" s="8">
         <v>236.7</v>
@@ -1560,7 +1554,7 @@
         <v>235</v>
       </c>
       <c r="F35" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G35" s="20"/>
       <c r="H35" s="21"/>
@@ -1572,7 +1566,7 @@
         <v>18</v>
       </c>
       <c r="B36" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C36" s="13">
         <v>225.79</v>
@@ -1585,7 +1579,7 @@
         <v>225.42000000000002</v>
       </c>
       <c r="F36" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G36" s="24"/>
       <c r="H36" s="21"/>
@@ -1597,7 +1591,7 @@
         <v>19</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C37" s="14">
         <v>216</v>
@@ -1620,7 +1614,7 @@
         <v>20</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C38" s="7">
         <v>209.9</v>
@@ -1643,7 +1637,7 @@
         <v>21</v>
       </c>
       <c r="B39" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C39" s="11">
         <v>214.7</v>
@@ -1656,7 +1650,7 @@
         <v>210.35</v>
       </c>
       <c r="F39" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G39" s="22"/>
       <c r="H39" s="21"/>
@@ -1668,7 +1662,7 @@
         <v>21</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C40" s="11">
         <v>214.7</v>
@@ -1681,7 +1675,7 @@
         <v>210.35</v>
       </c>
       <c r="F40" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G40" s="22"/>
       <c r="H40" s="23"/>
@@ -1689,10 +1683,10 @@
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B41" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C41" s="7">
         <v>218.2</v>
@@ -1705,7 +1699,7 @@
         <v>217.25</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G41" s="20"/>
       <c r="H41" s="23"/>
@@ -1713,10 +1707,10 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B42" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C42" s="7">
         <v>217.8</v>
@@ -1729,7 +1723,7 @@
         <v>216.8</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G42" s="20"/>
       <c r="H42" s="23"/>
@@ -1737,10 +1731,10 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C43" s="7">
         <v>217.8</v>
@@ -1753,7 +1747,7 @@
         <v>216.8</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G43" s="20"/>
       <c r="H43" s="23"/>
@@ -1761,10 +1755,10 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C44" s="8">
         <v>231.7</v>
@@ -1777,7 +1771,7 @@
         <v>229.35</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G44" s="20"/>
       <c r="H44" s="23"/>
@@ -1785,10 +1779,10 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C45" s="7">
         <v>216</v>
@@ -1801,7 +1795,7 @@
         <v>212.25</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G45" s="20"/>
       <c r="H45" s="23"/>
@@ -1809,10 +1803,10 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C46" s="8">
         <v>233.96</v>
@@ -1825,7 +1819,7 @@
         <v>230.48000000000002</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G46" s="20"/>
       <c r="H46" s="23"/>
@@ -1833,10 +1827,10 @@
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C47" s="7">
         <v>219</v>
@@ -1849,7 +1843,7 @@
         <v>217.4</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G47" s="20"/>
       <c r="H47" s="23"/>
@@ -1857,10 +1851,10 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C48" s="7">
         <v>223.036</v>
@@ -1878,10 +1872,10 @@
     </row>
     <row r="49" spans="1:9">
       <c r="A49" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C49" s="11">
         <v>214.7</v>
@@ -1894,7 +1888,7 @@
         <v>210.35</v>
       </c>
       <c r="F49" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G49" s="22"/>
       <c r="H49" s="23"/>
@@ -1902,10 +1896,10 @@
     </row>
     <row r="50" spans="1:9" ht="15" thickBot="1">
       <c r="A50" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C50" s="11">
         <v>214.7</v>
@@ -1918,7 +1912,7 @@
         <v>210.35</v>
       </c>
       <c r="F50" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G50" s="22"/>
       <c r="H50" s="23"/>
@@ -1926,13 +1920,13 @@
     </row>
     <row r="51" spans="1:9" ht="15" thickBot="1">
       <c r="A51" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F51" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G51" s="25"/>
       <c r="H51" s="23"/>
@@ -1940,13 +1934,13 @@
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1">
       <c r="A52" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F52" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G52" s="25"/>
       <c r="H52" s="23"/>
@@ -1954,13 +1948,13 @@
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1">
       <c r="A53" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B53" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F53" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G53" s="25"/>
       <c r="H53" s="23"/>
@@ -1968,13 +1962,13 @@
     </row>
     <row r="54" spans="1:9" ht="15" thickBot="1">
       <c r="A54" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B54" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F54" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="G54" s="25"/>
       <c r="H54" s="23"/>
@@ -1993,7 +1987,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9851237-01A2-4A74-AEF5-AB1CB64C8E21}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="A28" workbookViewId="0">
       <selection activeCell="H51" sqref="H51"/>
     </sheetView>
   </sheetViews>
@@ -2007,10 +2001,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>36</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2030,7 +2024,7 @@
         <v>216.65</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="4" spans="1:3">
@@ -2041,7 +2035,7 @@
         <v>216.65</v>
       </c>
       <c r="C4" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:3">
@@ -2052,7 +2046,7 @@
         <v>216.65</v>
       </c>
       <c r="C5" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:3">
@@ -2063,7 +2057,7 @@
         <v>208.8</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:3">
@@ -2074,7 +2068,7 @@
         <v>217.25</v>
       </c>
       <c r="C7" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:3">
@@ -2103,7 +2097,7 @@
         <v>210.35</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:3">
@@ -2114,7 +2108,7 @@
         <v>210.35</v>
       </c>
       <c r="C11" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="12" spans="1:3">
@@ -2125,7 +2119,7 @@
         <v>225.5</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:3">
@@ -2136,7 +2130,7 @@
         <v>221</v>
       </c>
       <c r="C13" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:3">
@@ -2147,7 +2141,7 @@
         <v>219.33999999999997</v>
       </c>
       <c r="C14" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="15" spans="1:3">
@@ -2158,7 +2152,7 @@
         <v>217.75</v>
       </c>
       <c r="C15" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="16" spans="1:3">
@@ -2169,7 +2163,7 @@
         <v>217.75</v>
       </c>
       <c r="C16" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="17" spans="1:3">
@@ -2180,7 +2174,7 @@
         <v>225.5</v>
       </c>
       <c r="C17" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="18" spans="1:3">
@@ -2191,7 +2185,7 @@
         <v>213</v>
       </c>
       <c r="C18" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="19" spans="1:3">
@@ -2202,7 +2196,7 @@
         <v>211.89999999999998</v>
       </c>
       <c r="C19" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="1:3">
@@ -2213,7 +2207,7 @@
         <v>211.89999999999998</v>
       </c>
       <c r="C20" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:3">
@@ -2224,7 +2218,7 @@
         <v>209.75</v>
       </c>
       <c r="C21" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="22" spans="1:3">
@@ -2235,7 +2229,7 @@
         <v>209.75</v>
       </c>
       <c r="C22" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="23" spans="1:3">
@@ -2246,7 +2240,7 @@
         <v>203.55</v>
       </c>
       <c r="C23" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="24" spans="1:3">
@@ -2257,7 +2251,7 @@
         <v>217.25</v>
       </c>
       <c r="C24" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:3">
@@ -2268,7 +2262,7 @@
         <v>225.42000000000002</v>
       </c>
       <c r="C25" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:3">
@@ -2279,7 +2273,7 @@
         <v>233.23000000000002</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="27" spans="1:3">
@@ -2299,7 +2293,7 @@
         <v>238.25</v>
       </c>
       <c r="C28" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="29" spans="1:3">
@@ -2310,7 +2304,7 @@
         <v>238.25</v>
       </c>
       <c r="C29" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="30" spans="1:3">
@@ -2330,7 +2324,7 @@
         <v>235</v>
       </c>
       <c r="C31" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="32" spans="1:3">
@@ -2341,7 +2335,7 @@
         <v>235</v>
       </c>
       <c r="C32" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -2352,7 +2346,7 @@
         <v>235</v>
       </c>
       <c r="C33" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="34" spans="1:3">
@@ -2363,7 +2357,7 @@
         <v>235</v>
       </c>
       <c r="C34" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -2374,7 +2368,7 @@
         <v>235</v>
       </c>
       <c r="C35" s="15" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -2385,7 +2379,7 @@
         <v>225.42000000000002</v>
       </c>
       <c r="C36" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -2414,7 +2408,7 @@
         <v>210.35</v>
       </c>
       <c r="C39" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -2425,89 +2419,89 @@
         <v>210.35</v>
       </c>
       <c r="C40" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:3">
       <c r="A41" s="3" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B41">
         <v>217.25</v>
       </c>
       <c r="C41" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="42" spans="1:3">
       <c r="A42" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B42">
         <v>216.8</v>
       </c>
       <c r="C42" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="43" spans="1:3">
       <c r="A43" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B43">
         <v>216.8</v>
       </c>
       <c r="C43" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:3">
       <c r="A44" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B44">
         <v>229.35</v>
       </c>
       <c r="C44" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="45" spans="1:3">
       <c r="A45" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B45">
         <v>212.25</v>
       </c>
       <c r="C45" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="46" spans="1:3">
       <c r="A46" s="5" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B46">
         <v>230.48000000000002</v>
       </c>
       <c r="C46" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:3">
       <c r="A47" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B47">
         <v>217.4</v>
       </c>
       <c r="C47" s="16" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:3">
       <c r="A48" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B48">
         <v>220.55799999999999</v>
@@ -2515,56 +2509,56 @@
     </row>
     <row r="49" spans="1:3">
       <c r="A49" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B49">
         <v>210.35</v>
       </c>
       <c r="C49" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="50" spans="1:3" ht="15" thickBot="1">
       <c r="A50" s="10" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B50">
         <v>210.35</v>
       </c>
       <c r="C50" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="51" spans="1:3" ht="15" thickBot="1">
       <c r="A51" s="18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C51" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="52" spans="1:3" ht="15" thickBot="1">
       <c r="A52" s="18" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C52" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="15" thickBot="1">
       <c r="A53" s="18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C53" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="54" spans="1:3" ht="15" thickBot="1">
       <c r="A54" s="18" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C54" s="19" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -2574,10 +2568,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CEA1D91-F59B-49D5-B2F5-1C963B59F067}">
-  <dimension ref="A1:I22"/>
+  <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+      <selection activeCell="N5" sqref="N5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2586,43 +2580,51 @@
     <col min="2" max="2" width="15" customWidth="1"/>
     <col min="3" max="4" width="8.77734375" customWidth="1"/>
     <col min="9" max="9" width="15.88671875" customWidth="1"/>
+    <col min="10" max="10" width="26.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>34</v>
-      </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9">
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" s="3">
         <v>217.8</v>
@@ -2634,27 +2636,33 @@
         <v>216.65</v>
       </c>
       <c r="F2">
-        <f>E2-201.3</f>
+        <f t="shared" ref="F2:F22" si="0">E2-201.3</f>
         <v>15.349999999999994</v>
       </c>
       <c r="G2">
-        <f>C2-201.3</f>
+        <f t="shared" ref="G2:G22" si="1">C2-201.3</f>
         <v>16.5</v>
       </c>
       <c r="H2">
-        <f>D2-201.3</f>
+        <f t="shared" ref="H2:H22" si="2">D2-201.3</f>
         <v>14.199999999999989</v>
       </c>
       <c r="I2" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="K2">
+        <v>15.349999999999994</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C3" s="7">
         <v>217.8</v>
@@ -2666,27 +2674,33 @@
         <v>216.65</v>
       </c>
       <c r="F3">
-        <f>E3-201.3</f>
+        <f t="shared" si="0"/>
         <v>15.349999999999994</v>
       </c>
       <c r="G3">
-        <f>C3-201.3</f>
+        <f t="shared" si="1"/>
         <v>16.5</v>
       </c>
       <c r="H3">
-        <f>D3-201.3</f>
+        <f t="shared" si="2"/>
         <v>14.199999999999989</v>
       </c>
       <c r="I3" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="K3">
+        <v>15.349999999999994</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4" s="3" t="s">
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C4" s="7">
         <v>216.3</v>
@@ -2698,27 +2712,33 @@
         <v>208.8</v>
       </c>
       <c r="F4">
-        <f>E4-201.3</f>
+        <f t="shared" si="0"/>
         <v>7.5</v>
       </c>
       <c r="G4">
-        <f>C4-201.3</f>
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
       <c r="H4">
-        <f>D4-201.3</f>
+        <f t="shared" si="2"/>
         <v>0</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K4">
+        <v>7.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5" s="3" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C5" s="7">
         <v>218.5</v>
@@ -2730,27 +2750,33 @@
         <v>217.25</v>
       </c>
       <c r="F5">
-        <f>E5-201.3</f>
+        <f t="shared" si="0"/>
         <v>15.949999999999989</v>
       </c>
       <c r="G5">
-        <f>C5-201.3</f>
+        <f t="shared" si="1"/>
         <v>17.199999999999989</v>
       </c>
       <c r="H5">
-        <f>D5-201.3</f>
+        <f t="shared" si="2"/>
         <v>14.699999999999989</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K5">
+        <v>15.949999999999989</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6" s="6" t="s">
         <v>8</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C6" s="9">
         <v>214.7</v>
@@ -2762,27 +2788,33 @@
         <v>210.35</v>
       </c>
       <c r="F6">
-        <f>E6-201.3</f>
+        <f t="shared" si="0"/>
         <v>9.0499999999999829</v>
       </c>
       <c r="G6">
-        <f>C6-201.3</f>
+        <f t="shared" si="1"/>
         <v>13.399999999999977</v>
       </c>
       <c r="H6">
-        <f>D6-201.3</f>
+        <f t="shared" si="2"/>
         <v>4.6999999999999886</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="K6">
+        <v>9.0499999999999829</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11">
       <c r="A7" s="6" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C7" s="9">
         <v>227</v>
@@ -2794,27 +2826,33 @@
         <v>217.75</v>
       </c>
       <c r="F7">
-        <f>E7-201.3</f>
+        <f t="shared" si="0"/>
         <v>16.449999999999989</v>
       </c>
       <c r="G7">
-        <f>C7-201.3</f>
+        <f t="shared" si="1"/>
         <v>25.699999999999989</v>
       </c>
       <c r="H7">
-        <f>D7-201.3</f>
+        <f t="shared" si="2"/>
         <v>7.1999999999999886</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="K7">
+        <v>16.449999999999989</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11">
       <c r="A8" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C8" s="8">
         <v>226</v>
@@ -2826,27 +2864,33 @@
         <v>225.5</v>
       </c>
       <c r="F8">
-        <f>E8-201.3</f>
+        <f t="shared" si="0"/>
         <v>24.199999999999989</v>
       </c>
       <c r="G8">
-        <f>C8-201.3</f>
+        <f t="shared" si="1"/>
         <v>24.699999999999989</v>
       </c>
       <c r="H8">
-        <f>D8-201.3</f>
+        <f t="shared" si="2"/>
         <v>1.6999999999999886</v>
       </c>
       <c r="I8" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J8" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="K8">
+        <v>24.199999999999989</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11">
       <c r="A9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="7">
         <v>218.2</v>
@@ -2858,27 +2902,33 @@
         <v>217.25</v>
       </c>
       <c r="F9">
-        <f>E9-201.3</f>
+        <f t="shared" si="0"/>
         <v>15.949999999999989</v>
       </c>
       <c r="G9">
-        <f>C9-201.3</f>
+        <f t="shared" si="1"/>
         <v>16.899999999999977</v>
       </c>
       <c r="H9">
-        <f>D9-201.3</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I9" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="K9">
+        <v>15.949999999999989</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11">
       <c r="A10" s="5" t="s">
         <v>12</v>
       </c>
       <c r="B10" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10" s="8">
         <v>225.79</v>
@@ -2890,27 +2940,33 @@
         <v>225.42000000000002</v>
       </c>
       <c r="F10">
-        <f>E10-201.3</f>
+        <f t="shared" si="0"/>
         <v>24.120000000000005</v>
       </c>
       <c r="G10">
-        <f>C10-201.3</f>
+        <f t="shared" si="1"/>
         <v>24.489999999999981</v>
       </c>
       <c r="H10">
-        <f>D10-201.3</f>
+        <f t="shared" si="2"/>
         <v>23.75</v>
       </c>
       <c r="I10" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J10" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="K10">
+        <v>24.120000000000005</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11">
       <c r="A11" s="5" t="s">
         <v>13</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C11" s="8">
         <v>233.96</v>
@@ -2922,27 +2978,33 @@
         <v>233.23000000000002</v>
       </c>
       <c r="F11">
-        <f>E11-201.3</f>
+        <f t="shared" si="0"/>
         <v>31.930000000000007</v>
       </c>
       <c r="G11">
-        <f>C11-201.3</f>
+        <f t="shared" si="1"/>
         <v>32.659999999999997</v>
       </c>
       <c r="H11">
-        <f>D11-201.3</f>
+        <f t="shared" si="2"/>
         <v>31.199999999999989</v>
       </c>
       <c r="I11" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="K11">
+        <v>31.930000000000007</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11">
       <c r="A12" s="6" t="s">
         <v>15</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C12" s="9">
         <v>239.5</v>
@@ -2954,27 +3016,33 @@
         <v>238.25</v>
       </c>
       <c r="F12">
-        <f>E12-201.3</f>
+        <f t="shared" si="0"/>
         <v>36.949999999999989</v>
       </c>
       <c r="G12">
-        <f>C12-201.3</f>
+        <f t="shared" si="1"/>
         <v>38.199999999999989</v>
       </c>
       <c r="H12">
-        <f>D12-201.3</f>
+        <f t="shared" si="2"/>
         <v>35.699999999999989</v>
       </c>
       <c r="I12" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J12" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="K12">
+        <v>36.949999999999989</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C13" s="8">
         <v>236.7</v>
@@ -2986,27 +3054,33 @@
         <v>235</v>
       </c>
       <c r="F13">
-        <f>E13-201.3</f>
+        <f t="shared" si="0"/>
         <v>33.699999999999989</v>
       </c>
       <c r="G13">
-        <f>C13-201.3</f>
+        <f t="shared" si="1"/>
         <v>35.399999999999977</v>
       </c>
       <c r="H13">
-        <f>D13-201.3</f>
+        <f t="shared" si="2"/>
         <v>32</v>
       </c>
       <c r="I13" s="15" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="K13">
+        <v>33.699999999999989</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
       <c r="A14" s="12" t="s">
         <v>18</v>
       </c>
       <c r="B14" s="12" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C14" s="13">
         <v>225.79</v>
@@ -3018,27 +3092,33 @@
         <v>225.42000000000002</v>
       </c>
       <c r="F14">
-        <f>E14-201.3</f>
+        <f t="shared" si="0"/>
         <v>24.120000000000005</v>
       </c>
       <c r="G14">
-        <f>C14-201.3</f>
+        <f t="shared" si="1"/>
         <v>24.489999999999981</v>
       </c>
       <c r="H14">
-        <f>D14-201.3</f>
+        <f t="shared" si="2"/>
         <v>23.75</v>
       </c>
       <c r="I14" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="K14">
+        <v>24.120000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B15" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C15" s="11">
         <v>214.7</v>
@@ -3050,27 +3130,33 @@
         <v>210.35</v>
       </c>
       <c r="F15">
-        <f>E15-201.3</f>
+        <f t="shared" si="0"/>
         <v>9.0499999999999829</v>
       </c>
       <c r="G15">
-        <f>C15-201.3</f>
+        <f t="shared" si="1"/>
         <v>13.399999999999977</v>
       </c>
       <c r="H15">
-        <f>D15-201.3</f>
+        <f t="shared" si="2"/>
         <v>4.6999999999999886</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J15" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="K15">
+        <v>9.0499999999999829</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11">
       <c r="A16" s="3" t="s">
-        <v>22</v>
+        <v>34</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C16" s="7">
         <v>218.2</v>
@@ -3082,27 +3168,33 @@
         <v>217.25</v>
       </c>
       <c r="F16">
-        <f>E16-201.3</f>
+        <f t="shared" si="0"/>
         <v>15.949999999999989</v>
       </c>
       <c r="G16">
-        <f>C16-201.3</f>
+        <f t="shared" si="1"/>
         <v>16.899999999999977</v>
       </c>
       <c r="H16">
-        <f>D16-201.3</f>
+        <f t="shared" si="2"/>
         <v>15</v>
       </c>
       <c r="I16" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="17" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="K16">
+        <v>15.949999999999989</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11">
       <c r="A17" s="3" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C17" s="7">
         <v>217.8</v>
@@ -3114,27 +3206,33 @@
         <v>216.8</v>
       </c>
       <c r="F17">
-        <f>E17-201.3</f>
+        <f t="shared" si="0"/>
         <v>15.5</v>
       </c>
       <c r="G17">
-        <f>C17-201.3</f>
+        <f t="shared" si="1"/>
         <v>16.5</v>
       </c>
       <c r="H17">
-        <f>D17-201.3</f>
+        <f t="shared" si="2"/>
         <v>14.5</v>
       </c>
       <c r="I17" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="K17">
+        <v>15.5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11">
       <c r="A18" s="5" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C18" s="8">
         <v>231.7</v>
@@ -3146,27 +3244,33 @@
         <v>229.35</v>
       </c>
       <c r="F18">
-        <f>E18-201.3</f>
+        <f t="shared" si="0"/>
         <v>28.049999999999983</v>
       </c>
       <c r="G18">
-        <f>C18-201.3</f>
+        <f t="shared" si="1"/>
         <v>30.399999999999977</v>
       </c>
       <c r="H18">
-        <f>D18-201.3</f>
+        <f t="shared" si="2"/>
         <v>25.699999999999989</v>
       </c>
       <c r="I18" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9">
+        <v>37</v>
+      </c>
+      <c r="J18" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="K18">
+        <v>28.049999999999983</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11">
       <c r="A19" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C19" s="7">
         <v>216</v>
@@ -3178,27 +3282,33 @@
         <v>212.25</v>
       </c>
       <c r="F19">
-        <f>E19-201.3</f>
+        <f t="shared" si="0"/>
         <v>10.949999999999989</v>
       </c>
       <c r="G19">
-        <f>C19-201.3</f>
+        <f t="shared" si="1"/>
         <v>14.699999999999989</v>
       </c>
       <c r="H19">
-        <f>D19-201.3</f>
+        <f t="shared" si="2"/>
         <v>7.1999999999999886</v>
       </c>
       <c r="I19" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="20" spans="1:9">
-      <c r="A20" s="28" t="s">
-        <v>26</v>
+        <v>37</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K19">
+        <v>10.949999999999989</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11">
+      <c r="A20" s="5" t="s">
+        <v>25</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C20" s="8">
         <v>233.96</v>
@@ -3210,27 +3320,33 @@
         <v>230.48000000000002</v>
       </c>
       <c r="F20">
-        <f>E20-201.3</f>
+        <f t="shared" si="0"/>
         <v>29.180000000000007</v>
       </c>
       <c r="G20">
-        <f>C20-201.3</f>
+        <f t="shared" si="1"/>
         <v>32.659999999999997</v>
       </c>
       <c r="H20">
-        <f>D20-201.3</f>
+        <f t="shared" si="2"/>
         <v>25.699999999999989</v>
       </c>
       <c r="I20" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="1:9">
-      <c r="A21" s="27" t="s">
-        <v>27</v>
+        <v>37</v>
+      </c>
+      <c r="J20" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="K20">
+        <v>29.180000000000007</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11">
+      <c r="A21" s="3" t="s">
+        <v>26</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C21" s="7">
         <v>219</v>
@@ -3242,27 +3358,33 @@
         <v>217.4</v>
       </c>
       <c r="F21">
-        <f>E21-201.3</f>
+        <f t="shared" si="0"/>
         <v>16.099999999999994</v>
       </c>
       <c r="G21">
-        <f>C21-201.3</f>
+        <f t="shared" si="1"/>
         <v>17.699999999999989</v>
       </c>
       <c r="H21">
-        <f>D21-201.3</f>
+        <f t="shared" si="2"/>
         <v>14.5</v>
       </c>
       <c r="I21" s="16" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="26" t="s">
-        <v>29</v>
+        <v>37</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21">
+        <v>16.099999999999994</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11">
+      <c r="A22" s="10" t="s">
+        <v>28</v>
       </c>
       <c r="B22" s="10" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C22" s="11">
         <v>214.7</v>
@@ -3274,19 +3396,25 @@
         <v>210.35</v>
       </c>
       <c r="F22">
-        <f>E22-201.3</f>
+        <f t="shared" si="0"/>
         <v>9.0499999999999829</v>
       </c>
       <c r="G22">
-        <f>C22-201.3</f>
+        <f t="shared" si="1"/>
         <v>13.399999999999977</v>
       </c>
       <c r="H22">
-        <f>D22-201.3</f>
+        <f t="shared" si="2"/>
         <v>4.6999999999999886</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
+      </c>
+      <c r="J22" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="K22">
+        <v>9.0499999999999829</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Work last couple days
</commit_message>
<xml_diff>
--- a/BEAST2/Ptero's/Data/Ptero ages.xlsx
+++ b/BEAST2/Ptero's/Data/Ptero ages.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Joël\Documents\GitHub\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\revbayes-v1.2.1-win64\revbayes-v1.2.1\Files\PterosaurPhylogeny\BEAST2\Ptero's\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBBB0B1-0A62-44EC-9218-D4526D6F1947}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{417837EF-E1F3-4619-AF1D-723A84A2BE1C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-12624" yWindow="5076" windowWidth="19704" windowHeight="15840" xr2:uid="{D1360FA9-3365-40CC-8225-CD928C39C5E1}"/>
+    <workbookView minimized="1" xWindow="864" yWindow="1056" windowWidth="15156" windowHeight="10536" xr2:uid="{D1360FA9-3365-40CC-8225-CD928C39C5E1}"/>
   </bookViews>
   <sheets>
     <sheet name="Raw(ish) age data" sheetId="1" r:id="rId1"/>
     <sheet name="Data for input into BEAST2" sheetId="2" r:id="rId2"/>
     <sheet name="Data no dupes" sheetId="3" r:id="rId3"/>
+    <sheet name="Only age data" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="55">
   <si>
     <t>accepted_name</t>
   </si>
@@ -176,6 +177,33 @@
   </si>
   <si>
     <t>med_hei</t>
+  </si>
+  <si>
+    <t>Campylognathoides liasicus</t>
+  </si>
+  <si>
+    <t>Campylognathoides zitteli</t>
+  </si>
+  <si>
+    <t>Dorygnathus banthensis</t>
+  </si>
+  <si>
+    <t>Eudimorphodon cromptonellus</t>
+  </si>
+  <si>
+    <t>Eudimorphodon rosenfeldi</t>
+  </si>
+  <si>
+    <t>Parapsicephalus purdoni</t>
+  </si>
+  <si>
+    <t>Rhamphinion jenkinsi</t>
+  </si>
+  <si>
+    <t>Dorygnathus purdoni</t>
+  </si>
+  <si>
+    <t>Areripedctylus dehmi</t>
   </si>
 </sst>
 </file>
@@ -221,7 +249,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="16">
+  <fills count="17">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -312,6 +340,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -370,13 +404,11 @@
     <xf numFmtId="0" fontId="1" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="12" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="14" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="12" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="15" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="16" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -392,7 +424,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -690,8 +722,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D336B04-D74B-4DEC-B807-60D1529292D8}">
   <dimension ref="A1:J54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A57" sqref="A57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -1932,22 +1964,25 @@
       <c r="B51" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C51" s="26">
+      <c r="C51" s="25"/>
+      <c r="D51" s="25"/>
+      <c r="E51" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F51" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G51" s="25">
         <v>184.2</v>
       </c>
-      <c r="D51" s="26">
+      <c r="H51" s="25">
         <v>168.2</v>
       </c>
-      <c r="E51">
-        <f t="shared" si="0"/>
+      <c r="I51">
+        <f>MEDIAN(G51,H51)</f>
         <v>176.2</v>
       </c>
-      <c r="F51" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G51" s="25"/>
-      <c r="H51" s="23"/>
-      <c r="I51" s="23"/>
     </row>
     <row r="52" spans="1:9" ht="15" thickBot="1">
       <c r="A52" s="18" t="s">
@@ -1956,22 +1991,25 @@
       <c r="B52" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C52" s="26">
+      <c r="C52" s="25"/>
+      <c r="D52" s="25"/>
+      <c r="E52" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F52" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G52" s="25">
         <v>161.5</v>
       </c>
-      <c r="D52" s="26">
+      <c r="H52" s="25">
         <v>154.80000000000001</v>
       </c>
-      <c r="E52">
-        <f t="shared" si="0"/>
+      <c r="I52">
+        <f>MEDIAN(G52,H52)</f>
         <v>158.15</v>
       </c>
-      <c r="F52" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G52" s="25"/>
-      <c r="H52" s="23"/>
-      <c r="I52" s="23"/>
     </row>
     <row r="53" spans="1:9" ht="15" thickBot="1">
       <c r="A53" s="18" t="s">
@@ -1980,22 +2018,25 @@
       <c r="B53" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C53" s="26">
+      <c r="C53" s="25"/>
+      <c r="D53" s="25"/>
+      <c r="E53" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F53" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G53" s="25">
         <v>201.4</v>
       </c>
-      <c r="D53" s="26">
+      <c r="H53" s="25">
         <v>188</v>
       </c>
-      <c r="E53">
-        <f t="shared" si="0"/>
+      <c r="I53">
+        <f>MEDIAN(G53,H53)</f>
         <v>194.7</v>
       </c>
-      <c r="F53" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G53" s="25"/>
-      <c r="H53" s="23"/>
-      <c r="I53" s="23"/>
     </row>
     <row r="54" spans="1:9" ht="15" thickBot="1">
       <c r="A54" s="18" t="s">
@@ -2004,22 +2045,25 @@
       <c r="B54" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="C54" s="26">
+      <c r="C54" s="25"/>
+      <c r="D54" s="25"/>
+      <c r="E54" t="e">
+        <f t="shared" si="0"/>
+        <v>#NUM!</v>
+      </c>
+      <c r="F54" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="25">
         <v>154.80000000000001</v>
       </c>
-      <c r="D54" s="26">
+      <c r="H54" s="25">
         <v>145</v>
       </c>
-      <c r="E54">
-        <f t="shared" si="0"/>
+      <c r="I54">
+        <f>MEDIAN(G54,H54)</f>
         <v>149.9</v>
       </c>
-      <c r="F54" s="19" t="s">
-        <v>37</v>
-      </c>
-      <c r="G54" s="25"/>
-      <c r="H54" s="23"/>
-      <c r="I54" s="23"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="G2:I50">
@@ -2034,8 +2078,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9851237-01A2-4A74-AEF5-AB1CB64C8E21}">
   <dimension ref="A1:C54"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="H51" sqref="H51"/>
+    <sheetView topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="I48" sqref="I48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2580,6 +2624,9 @@
       <c r="A51" s="18" t="s">
         <v>38</v>
       </c>
+      <c r="B51">
+        <v>176.2</v>
+      </c>
       <c r="C51" s="19" t="s">
         <v>37</v>
       </c>
@@ -2588,6 +2635,9 @@
       <c r="A52" s="18" t="s">
         <v>39</v>
       </c>
+      <c r="B52">
+        <v>158.15</v>
+      </c>
       <c r="C52" s="19" t="s">
         <v>37</v>
       </c>
@@ -2596,6 +2646,9 @@
       <c r="A53" s="18" t="s">
         <v>40</v>
       </c>
+      <c r="B53">
+        <v>194.7</v>
+      </c>
       <c r="C53" s="19" t="s">
         <v>37</v>
       </c>
@@ -2603,6 +2656,9 @@
     <row r="54" spans="1:3" ht="15" thickBot="1">
       <c r="A54" s="18" t="s">
         <v>41</v>
+      </c>
+      <c r="B54">
+        <v>149.9</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>37</v>
@@ -2618,7 +2674,7 @@
   <dimension ref="A1:K22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -3470,4 +3526,75 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C6AE50A-C2BE-4C64-A219-6E839C16AC14}">
+  <dimension ref="A1:A10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4"/>
+  <cols>
+    <col min="1" max="1" width="26.5546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" s="26" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="26" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="26" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="26" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="26" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="26" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="26" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="26" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="26" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A10">
+    <sortCondition ref="A1:A10"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>